<commit_message>
refactored jobs_site class methods to jobs_queue
</commit_message>
<xml_diff>
--- a/jobboard_info.xlsx
+++ b/jobboard_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913F1A5B-EB32-48D0-ADE6-0E7690A650C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBD9C8E-32DF-4D9C-A677-0CFC05206B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="job_sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="203">
   <si>
     <t>name</t>
   </si>
@@ -638,6 +638,18 @@
   <si>
     <t>https://www.dai.com/careers/search.html?keywords=Evaluation&amp;location=&amp;functional_area=
 https://phf.tbe.taleo.net/phf04/ats/careers/searchResults.jsp?org=DAINC&amp;cws=1</t>
+  </si>
+  <si>
+    <t>hta consulting</t>
+  </si>
+  <si>
+    <t>http://www.htaconsulting.com/blog/</t>
+  </si>
+  <si>
+    <t>Research &amp; evaluation firm in bay area. Looks like good work.</t>
+  </si>
+  <si>
+    <t>Berkeley</t>
   </si>
 </sst>
 </file>
@@ -974,10 +986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,6 +2637,38 @@
       </c>
       <c r="J51" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" s="1">
+        <v>20</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2803,10 +2848,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C67817-6EEA-4F49-A445-F6800BBA50C9}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2926,6 +2971,14 @@
         <v>158</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
renamed files & objects for clarity. running correctly. fixed  warning
</commit_message>
<xml_diff>
--- a/jobboard_info.xlsx
+++ b/jobboard_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBD9C8E-32DF-4D9C-A677-0CFC05206B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A786B49C-2E2D-4FCF-A88F-97B75EFB29DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="job_sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="209">
   <si>
     <t>name</t>
   </si>
@@ -650,13 +650,31 @@
   </si>
   <si>
     <t>Berkeley</t>
+  </si>
+  <si>
+    <t>acumen</t>
+  </si>
+  <si>
+    <t>https://www.acumenllc.com/careers.html#accordion-Team1%20.item-1</t>
+  </si>
+  <si>
+    <t>Research &amp; evalation firm for policymaking</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Burlingame</t>
+  </si>
+  <si>
+    <t>1,8,14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +696,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -696,18 +722,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -986,7 +1015,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1041,7 +1070,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>45</v>
@@ -2669,6 +2698,38 @@
       </c>
       <c r="J52" s="1">
         <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="1">
+        <v>20</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2677,6 +2738,7 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" location="results/5f7632188a269a919fd9419b?kw=&amp;loc=&amp;page_num=1" display="https://jobs.humentum.org/search/#results/5f7632188a269a919fd9419b?kw=&amp;loc=&amp;page_num=1" xr:uid="{294E73C3-894E-4559-9FC7-CD43CA94AF6E}"/>
+    <hyperlink ref="C53" r:id="rId2" location="accordion-Team1%20.item-1" xr:uid="{015A9B52-AB28-4F71-9731-5E2F5CE31D70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2848,10 +2910,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C67817-6EEA-4F49-A445-F6800BBA50C9}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,6 +3041,14 @@
         <v>202</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated readme with todo list
</commit_message>
<xml_diff>
--- a/jobboard_info.xlsx
+++ b/jobboard_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A786B49C-2E2D-4FCF-A88F-97B75EFB29DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59088201-54DE-4EF6-B24E-1252A99A648B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="232">
   <si>
     <t>name</t>
   </si>
@@ -668,6 +668,79 @@
   </si>
   <si>
     <t>1,8,14</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=monitoring+and+evaluation+jobs+washington+dc&amp;rlz=1C1GCEA_enUS808US808&amp;oq=monitoring+and+evaluation+jobs+washington+dc&amp;aqs=chrome..69i57j69i60.7551j0j1&amp;sourceid=chrome&amp;ie=UTF-8&amp;ibp=htl;jobs&amp;sa=X&amp;ved=2ahUKEwiey-qryKjsAhVvCjQIHfYVBDkQiYsCKAJ6BAgMECg&amp;sxsrf=ALeKk02QhDrDaiK6sD-Uj4av3mY4GQAz2Q:1602282738861#htivrt=jobs&amp;htidocid=IX48xdfelX9mKorAAAAAAA%3D%3D&amp;fpstate=tldetail</t>
+  </si>
+  <si>
+    <t>M&amp;E jobs in DC</t>
+  </si>
+  <si>
+    <t>https://cipe.applytojob.com/apply/</t>
+  </si>
+  <si>
+    <t>Center for International Private Enterprise</t>
+  </si>
+  <si>
+    <t>The Center for International Private Enterprise (CIPE) strengthens democracy around the globe through private enterprise and market-oriented reform. CIPE is one of the four core institutes of the National Endowment for Democracy.</t>
+  </si>
+  <si>
+    <t>The National Democratic Institute, or National Democratic Institute for International Affairs, is a non-partisan, non-profit organization that works with partners in developing countries to increase the effectiveness of democratic institutions. NDI is one of the four core institutes of the National Endowment for Democracy.</t>
+  </si>
+  <si>
+    <t>National Democratic Institute</t>
+  </si>
+  <si>
+    <t>https://ndi.secure.force.com/careers/ts2__JobSearch</t>
+  </si>
+  <si>
+    <t>american Center for International Labor Solidarity (ACILS)</t>
+  </si>
+  <si>
+    <t>https://www.solidaritycenter.org/who-we-are/jobs-internships/</t>
+  </si>
+  <si>
+    <t>The Solidarity Center is a non-profit organization aligned with the AFL-CIO labor federation. It is one of the core grantees of the National Endowment for Democracy.</t>
+  </si>
+  <si>
+    <t>International Republican Institute (IRI)</t>
+  </si>
+  <si>
+    <t>https://www.iri.org/work-with-us</t>
+  </si>
+  <si>
+    <t>Washington, DC nonprofit, nonpartisan organization committed to advancing freedom and democracy worldwide by helping political parties to become more issue-based and responsive, assisting citizens to participate in government planning, and working to increase the role of marginalized groups in the political process – including women and youth. one of the four core institutes of the National Endowment for Democracy.
+NOTE: Lists procurement opportunities. May like to return later to this.</t>
+  </si>
+  <si>
+    <t>Jefferson Consulting Group Careers</t>
+  </si>
+  <si>
+    <t>https://jobs.jobvite.com/jefferson/jobs</t>
+  </si>
+  <si>
+    <t>Jefferson provides strategic and operational services to federal agencies in program management, acquisition, human capital and training including USAID -- lots of M&amp;E opportunities</t>
+  </si>
+  <si>
+    <t>Edjoin</t>
+  </si>
+  <si>
+    <t>https://www.edjoin.org/Home/Jobs?keywords=Research&amp;searchType=all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+EDJOIN - The Nation's #1 Education Job Boardwww.edjoin.org
+Education jobs, education jobs in America, education jobs in United States, Teaching jobs, Teaching jobs in America, Teaching jobs in United States, Education</t>
+  </si>
+  <si>
+    <t>association of california school administrators (acsa)</t>
+  </si>
+  <si>
+    <t>ACSA is the largest umbrella association for school leaders in the United States, serving more than 17000 California educators.</t>
+  </si>
+  <si>
+    <t>https://careers.acsa.org/jobs/?keywords=Data
+https://careers.acsa.org/jobs/?keywords=&amp;category=digital&amp;category=program-specialist&amp;category=research-laboratory-non-laboratory&amp;category=research-support-laboratory-non-laboratory&amp;category=social-behavioral-sciences&amp;sort=</t>
   </si>
 </sst>
 </file>
@@ -726,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -734,6 +807,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1015,11 +1090,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1118,7 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1651,7 +1726,7 @@
       <c r="B20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -2730,6 +2805,262 @@
       </c>
       <c r="J53" s="1" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E54" s="1">
+        <v>10</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>2</v>
+      </c>
+      <c r="I54" s="1">
+        <v>2</v>
+      </c>
+      <c r="J54" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E55" s="1">
+        <v>20</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
+      </c>
+      <c r="H55" s="1">
+        <v>2</v>
+      </c>
+      <c r="I55" s="1">
+        <v>2</v>
+      </c>
+      <c r="J55" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="E56" s="1">
+        <v>20</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1">
+        <v>2</v>
+      </c>
+      <c r="I56" s="1">
+        <v>2</v>
+      </c>
+      <c r="J56" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E57" s="1">
+        <v>20</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
+      <c r="H57" s="1">
+        <v>2</v>
+      </c>
+      <c r="I57" s="1">
+        <v>2</v>
+      </c>
+      <c r="J57" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E58" s="1">
+        <v>50</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
+      <c r="H58" s="1">
+        <v>2</v>
+      </c>
+      <c r="I58" s="1">
+        <v>2</v>
+      </c>
+      <c r="J58" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E59" s="1">
+        <v>20</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <v>2</v>
+      </c>
+      <c r="J59" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E60" s="1">
+        <v>15</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E61" s="1">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2739,6 +3070,13 @@
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" location="results/5f7632188a269a919fd9419b?kw=&amp;loc=&amp;page_num=1" display="https://jobs.humentum.org/search/#results/5f7632188a269a919fd9419b?kw=&amp;loc=&amp;page_num=1" xr:uid="{294E73C3-894E-4559-9FC7-CD43CA94AF6E}"/>
     <hyperlink ref="C53" r:id="rId2" location="accordion-Team1%20.item-1" xr:uid="{015A9B52-AB28-4F71-9731-5E2F5CE31D70}"/>
+    <hyperlink ref="C20" r:id="rId3" location="htivrt=jobs&amp;htidocid=AEiQPiGPhk9Vy7hrAAAAAA%3D%3D&amp;fpstate=tldetail" display="https://www.google.com/search?q=monitoring+and+evaluation+jobs+california&amp;rlz=1C1GCEA_enUS808US808&amp;oq=monitoring+and+evaluation+jobs+&amp;aqs=chrome.1.69i59l3j0l2j69i60l3.4212j0j7&amp;sourceid=chrome&amp;ie=UTF-8&amp;ibp=htl;jobs&amp;sa=X&amp;ved=2ahUKEwik1aLXyJHsAhXzKX0KHdw_BeIQiYsCKAJ6BAgMECg&amp;sxsrf=ALeKk00ClfBYhG4tgcqVblxWrjSO2OssmQ:1601492555974#htivrt=jobs&amp;htidocid=AEiQPiGPhk9Vy7hrAAAAAA%3D%3D&amp;fpstate=tldetail" xr:uid="{9ADEE9F5-CAF2-4993-A099-D4D7DD6D5C48}"/>
+    <hyperlink ref="C54" r:id="rId4" location="htivrt=jobs&amp;htidocid=IX48xdfelX9mKorAAAAAAA%3D%3D&amp;fpstate=tldetail" display="https://www.google.com/search?q=monitoring+and+evaluation+jobs+washington+dc&amp;rlz=1C1GCEA_enUS808US808&amp;oq=monitoring+and+evaluation+jobs+washington+dc&amp;aqs=chrome..69i57j69i60.7551j0j1&amp;sourceid=chrome&amp;ie=UTF-8&amp;ibp=htl;jobs&amp;sa=X&amp;ved=2ahUKEwiey-qryKjsAhVvCjQIHfYVBDkQiYsCKAJ6BAgMECg&amp;sxsrf=ALeKk02QhDrDaiK6sD-Uj4av3mY4GQAz2Q:1602282738861#htivrt=jobs&amp;htidocid=IX48xdfelX9mKorAAAAAAA%3D%3D&amp;fpstate=tldetail" xr:uid="{2FF3FF9E-0179-4EB2-A847-5A994F842151}"/>
+    <hyperlink ref="C55" r:id="rId5" xr:uid="{5131CAA0-1115-4CA6-8C18-CF3D7C7391B9}"/>
+    <hyperlink ref="C56" r:id="rId6" xr:uid="{B9F7AFAD-5036-48FE-9BEA-763E8DE7F808}"/>
+    <hyperlink ref="C57" r:id="rId7" xr:uid="{E817039A-6612-4976-AC9B-2969C04F20B2}"/>
+    <hyperlink ref="C58" r:id="rId8" xr:uid="{D770099D-431E-4F2D-AE58-59DD5B7F686F}"/>
+    <hyperlink ref="C59" r:id="rId9" xr:uid="{E7E465D7-F7F6-4AF0-85EE-B0A46DFD98C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactored auxiliary print methods & fixed writing without records file
</commit_message>
<xml_diff>
--- a/jobboard_info.xlsx
+++ b/jobboard_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59088201-54DE-4EF6-B24E-1252A99A648B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607AADD1-B683-44F5-9059-F01A86EDE1E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="job_sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="255">
   <si>
     <t>name</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>https://www.progressivedatajobs.org/</t>
-  </si>
-  <si>
-    <t>https://www.idealist.org/en/jobs?functions=DATA_EVALUATION_ANALYSIS&amp;functions=DATABASE_ADMINISTRATION&amp;functions=TECHNOLOGY_IT&amp;functions=RESEARCH&amp;page=2&amp;q=&amp;searchMode=true</t>
   </si>
   <si>
     <t>https://www.edsurge.com/jobs?filters%5Bcategory%5D%5B0%5D=Operations&amp;filters%5Bcategory%5D%5B1%5D=Research&amp;filters%5Bcategory%5D%5B2%5D=Engineering&amp;is_v=1</t>
@@ -741,13 +738,99 @@
   <si>
     <t>https://careers.acsa.org/jobs/?keywords=Data
 https://careers.acsa.org/jobs/?keywords=&amp;category=digital&amp;category=program-specialist&amp;category=research-laboratory-non-laboratory&amp;category=research-support-laboratory-non-laboratory&amp;category=social-behavioral-sciences&amp;sort=</t>
+  </si>
+  <si>
+    <t>Gain Power</t>
+  </si>
+  <si>
+    <r>
+      <t>GAIN POWER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Directories, jobs, stories, resources, networking &amp; marketing for progressive nonprofits, Democratic campaigns, the Resistance movement,</t>
+    </r>
+  </si>
+  <si>
+    <t>https://careercenter.gainpower.org/jobs/?keywords=&amp;keywords_cache=data&amp;location=&amp;location_completion=&amp;location_type=&amp;location_text=&amp;location_autocomplete=true&amp;t731=600784&amp;t731=672522&amp;t731=600794&amp;t731=600796&amp;t731=600797</t>
+  </si>
+  <si>
+    <t>NPO</t>
+  </si>
+  <si>
+    <t>NPO.net provides free job searches and resume postings for job seekers to find their fit and fuel their passion. For those looking to propel their job search and careers forward.
+For nonprofits and socially minded business, we provide an easy to use platform for you to attract, identify, engage and hire high quality candidates who share your mission.</t>
+  </si>
+  <si>
+    <t>https://careers.npo.net/index.php?action=advanced_search&amp;page=search&amp;keywords=Data&amp;country=United+States&amp;state%5B%5D=&amp;city=&amp;zip=&amp;zip_radius=&amp;position_type=&amp;min_salary=&amp;max_salary=&amp;salary_type=</t>
+  </si>
+  <si>
+    <t>tech jobs for good</t>
+  </si>
+  <si>
+    <t>https://www.techjobsforgood.com/jobs/?q=&amp;job_function=Data+%2B+Analytics</t>
+  </si>
+  <si>
+    <t>Tech Jobs for Good helps organizations working on social and environmental issues hire tech talent looking for purposeful work.</t>
+  </si>
+  <si>
+    <t>https://boards.greenhouse.io/techco</t>
+  </si>
+  <si>
+    <t>tech co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tech co. is a platform for advocates to create, power, and cultivate communities at local and national levels. We provide mobilization and data tools to non-profits, issue advocacy groups, electoral groups, and corporate social impact teams. </t>
+  </si>
+  <si>
+    <t>talking points</t>
+  </si>
+  <si>
+    <t>https://talkingpts.org/our-team/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TalkingPoints is an education technology nonprofit with a mission to drive student success by using accessible technology to unlock the potential of family engagement in children’s education.
+Our multilingual technology platform connects and empowers families and teachers by using human and AI-powered, two-way translated communication and personalized content. </t>
+  </si>
+  <si>
+    <t>Data Fellowship</t>
+  </si>
+  <si>
+    <t>Delta Analytics</t>
+  </si>
+  <si>
+    <t>http://www.deltanalytics.org/fellowship-faq.html#countfellows</t>
+  </si>
+  <si>
+    <t>https://www.idealist.org/en/jobs?functions=DATA_EVALUATION_ANALYSIS&amp;functions=RESEARCH&amp;q=&amp;searchMode=true
+https://www.idealist.org/en/jobs?functions=DATA_EVALUATION_ANALYSIS&amp;functions=RESEARCH&amp;q=&amp;searchMode=true</t>
+  </si>
+  <si>
+    <t>council on foreign relations</t>
+  </si>
+  <si>
+    <t>https://www.cfr.org/career-opportunities/open-positions</t>
+  </si>
+  <si>
+    <t>The Council on Foreign Relations, founded in 1921, is a United States nonprofit think tank specializing in U.S. foreign policy and international affairs.</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>5,8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -769,14 +852,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -795,23 +870,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1090,11 +1159,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,48 +1182,48 @@
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" s="1">
         <v>6</v>
@@ -1180,13 +1249,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1">
         <v>6</v>
@@ -1212,13 +1281,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="1">
         <v>20</v>
@@ -1244,13 +1313,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1">
         <v>20</v>
@@ -1265,10 +1334,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1276,13 +1345,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1">
         <v>6</v>
@@ -1308,13 +1377,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="1">
         <v>20</v>
@@ -1340,13 +1409,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="1">
         <v>20</v>
@@ -1372,13 +1441,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="1">
         <v>6</v>
@@ -1404,13 +1473,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1">
         <v>20</v>
@@ -1425,10 +1494,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1436,13 +1505,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1">
         <v>6</v>
@@ -1468,13 +1537,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="1">
         <v>6</v>
@@ -1500,13 +1569,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="1">
         <v>20</v>
@@ -1521,10 +1590,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1532,13 +1601,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" s="1">
         <v>5</v>
@@ -1564,13 +1633,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" s="1">
         <v>6</v>
@@ -1596,13 +1665,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="1">
         <v>20</v>
@@ -1628,13 +1697,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
@@ -1660,13 +1729,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>100</v>
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E18" s="1">
         <v>20</v>
@@ -1692,13 +1761,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" s="1">
         <v>20</v>
@@ -1713,10 +1782,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1724,13 +1793,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>19</v>
+        <v>61</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -1756,13 +1825,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
@@ -1788,13 +1857,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
@@ -1820,13 +1889,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="1">
         <v>5</v>
@@ -1852,13 +1921,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="1">
         <v>11</v>
@@ -1884,13 +1953,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="1">
         <v>6</v>
@@ -1916,13 +1985,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="1">
         <v>20</v>
@@ -1948,13 +2017,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1">
         <v>6</v>
@@ -1980,13 +2049,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E28" s="1">
         <v>6</v>
@@ -2012,13 +2081,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
+        <v>249</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
@@ -2044,13 +2113,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="1">
         <v>5</v>
@@ -2076,13 +2145,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" s="1">
         <v>20</v>
@@ -2097,10 +2166,10 @@
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2108,13 +2177,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E32" s="1">
         <v>6</v>
@@ -2140,13 +2209,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E33" s="1">
         <v>6</v>
@@ -2172,13 +2241,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="1">
         <v>6</v>
@@ -2204,13 +2273,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E35" s="1">
         <v>6</v>
@@ -2236,13 +2305,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
@@ -2268,13 +2337,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E37" s="1">
         <v>20</v>
@@ -2300,13 +2369,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="E38" s="1">
         <v>20</v>
@@ -2321,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2332,13 +2401,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E39" s="1">
         <v>20</v>
@@ -2364,13 +2433,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E40" s="1">
         <v>20</v>
@@ -2382,13 +2451,13 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2396,13 +2465,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E41" s="1">
         <v>20</v>
@@ -2417,10 +2486,10 @@
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2428,13 +2497,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E42" s="1">
         <v>20</v>
@@ -2460,13 +2529,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E43" s="1">
         <v>20</v>
@@ -2492,13 +2561,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E44" s="1">
         <v>20</v>
@@ -2524,13 +2593,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E45" s="1">
         <v>9</v>
@@ -2556,13 +2625,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E46" s="1">
         <v>9</v>
@@ -2588,13 +2657,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E47" s="1">
         <v>15</v>
@@ -2620,13 +2689,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E48" s="1">
         <v>20</v>
@@ -2652,13 +2721,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E49" s="1">
         <v>20</v>
@@ -2684,13 +2753,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E50" s="1">
         <v>20</v>
@@ -2716,13 +2785,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="E51" s="1">
         <v>20</v>
@@ -2748,13 +2817,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="E52" s="1">
         <v>20</v>
@@ -2780,13 +2849,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="D53" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="E53" s="1">
         <v>20</v>
@@ -2801,10 +2870,10 @@
         <v>1</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2812,13 +2881,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E54" s="1">
         <v>10</v>
@@ -2844,13 +2913,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="E55" s="1">
         <v>20</v>
@@ -2876,13 +2945,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>214</v>
+      <c r="D56" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="E56" s="1">
         <v>20</v>
@@ -2908,13 +2977,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="D57" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="E57" s="1">
         <v>20</v>
@@ -2940,13 +3009,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="D58" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="E58" s="1">
         <v>50</v>
@@ -2972,13 +3041,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="D59" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E59" s="1">
         <v>20</v>
@@ -3004,13 +3073,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="E60" s="1">
         <v>15</v>
@@ -3036,13 +3105,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E61" s="1">
         <v>15</v>
@@ -3057,11 +3126,236 @@
         <v>1</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J61" s="1">
         <v>0</v>
       </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E62" s="1">
+        <v>10</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E63" s="1">
+        <v>10</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E64" s="1">
+        <v>10</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E65" s="1">
+        <v>20</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E66" s="1">
+        <v>20</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>1</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E67" s="1">
+        <v>60</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
+      <c r="J67" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E68" s="1">
+        <v>20</v>
+      </c>
+      <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="K68" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J43">
@@ -3077,6 +3371,8 @@
     <hyperlink ref="C57" r:id="rId7" xr:uid="{E817039A-6612-4976-AC9B-2969C04F20B2}"/>
     <hyperlink ref="C58" r:id="rId8" xr:uid="{D770099D-431E-4F2D-AE58-59DD5B7F686F}"/>
     <hyperlink ref="C59" r:id="rId9" xr:uid="{E7E465D7-F7F6-4AF0-85EE-B0A46DFD98C0}"/>
+    <hyperlink ref="C67" r:id="rId10" location="countfellows" xr:uid="{3A18ED2F-F5D8-47A3-9836-9776AE6B46EB}"/>
+    <hyperlink ref="C29" r:id="rId11" display="https://www.idealist.org/en/jobs?functions=DATA_EVALUATION_ANALYSIS&amp;functions=RESEARCH&amp;q=&amp;searchMode=true" xr:uid="{5E0E8BB8-1E86-465D-8A91-3BB2B03A1E6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3097,18 +3393,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>141</v>
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3116,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3124,7 +3420,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3132,7 +3428,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3155,10 +3451,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3166,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3174,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3182,7 +3478,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3190,7 +3486,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3198,7 +3494,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3206,7 +3502,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3214,7 +3510,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3222,7 +3518,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3230,7 +3526,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3238,7 +3534,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3261,10 +3557,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3272,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3280,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3288,7 +3584,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,7 +3592,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3304,7 +3600,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3312,7 +3608,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3320,7 +3616,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3328,7 +3624,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3336,7 +3632,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3344,7 +3640,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3352,7 +3648,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3360,7 +3656,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,7 +3664,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3376,7 +3672,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3384,7 +3680,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lowered constant & fixed urls
</commit_message>
<xml_diff>
--- a/jobboard_info.xlsx
+++ b/jobboard_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EFDD30-8FC2-44E3-B2D5-F177404463A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D5D362-9A38-4866-A617-6E84721C3A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,10 +627,6 @@
 https://jobs.humentum.org/job-category/other/</t>
   </si>
   <si>
-    <t>https://www.dai.com/careers/search.html?keywords=Evaluation&amp;location=&amp;functional_area=
-https://phf.tbe.taleo.net/phf04/ats/careers/searchResults.jsp?org=DAINC&amp;cws=1</t>
-  </si>
-  <si>
     <t>hta consulting</t>
   </si>
   <si>
@@ -824,6 +820,10 @@
   </si>
   <si>
     <t>https://recruiting.ultipro.com/tec1006teser/jobboard/18180d88-ced0-4361-bd09-d5eef66dab24/?q=data&amp;o=postedDateDesc</t>
+  </si>
+  <si>
+    <t>https://www.dai.com/careers/search.html?keywords=Evaluation&amp;location=&amp;functional_area=
+https://www.dai.com/careers/search.html?keywords=Data&amp;location=United+States</t>
   </si>
 </sst>
 </file>
@@ -1173,8 +1173,8 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,7 +1615,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>93</v>
@@ -2095,7 +2095,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>106</v>
@@ -2383,7 +2383,7 @@
         <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>26</v>
@@ -2415,7 +2415,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>115</v>
@@ -2828,13 +2828,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>198</v>
       </c>
       <c r="E52" s="1">
         <v>20</v>
@@ -2860,13 +2860,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="E53" s="1">
         <v>20</v>
@@ -2881,10 +2881,10 @@
         <v>1</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2895,10 +2895,10 @@
         <v>59</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="E54" s="1">
         <v>10</v>
@@ -2924,13 +2924,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E55" s="1">
         <v>20</v>
@@ -2956,13 +2956,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E56" s="1">
         <v>20</v>
@@ -2988,13 +2988,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="E57" s="1">
         <v>20</v>
@@ -3020,13 +3020,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="E58" s="1">
         <v>50</v>
@@ -3052,13 +3052,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="E59" s="1">
         <v>20</v>
@@ -3084,13 +3084,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E60" s="1">
         <v>15</v>
@@ -3116,13 +3116,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="E61" s="1">
         <v>15</v>
@@ -3137,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J61" s="1">
         <v>0</v>
@@ -3148,13 +3148,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E62" s="1">
         <v>10</v>
@@ -3180,13 +3180,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="E63" s="1">
         <v>10</v>
@@ -3212,13 +3212,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E64" s="1">
         <v>10</v>
@@ -3244,13 +3244,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="E65" s="1">
         <v>20</v>
@@ -3276,13 +3276,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="E66" s="1">
         <v>20</v>
@@ -3308,13 +3308,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="D67" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E67" s="1">
         <v>60</v>
@@ -3340,13 +3340,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="E68" s="1">
         <v>20</v>
@@ -3361,10 +3361,10 @@
         <v>1</v>
       </c>
       <c r="I68" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="K68" s="1"/>
     </row>
@@ -3685,7 +3685,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3693,7 +3693,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>